<commit_message>
added labels to plots for red/blue lines
</commit_message>
<xml_diff>
--- a/inst/checklist.xlsx
+++ b/inst/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustinfife/Documents/RPackages/flexplavaan/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B40B47-9D16-2C4C-9A7C-DBEADC10014A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286093A3-9CF5-7945-ABFF-965D3FDC841C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28040" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{3781B20C-7E78-454B-86B5-5C89B4C55752}"/>
+    <workbookView xWindow="-39500" yWindow="720" windowWidth="38400" windowHeight="21140" xr2:uid="{3781B20C-7E78-454B-86B5-5C89B4C55752}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,35 +114,272 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="18">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,119 +696,128 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5916984-94A8-E344-85B5-574930A8EACE}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="18" t="s">
         <v>0</v>
       </c>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="10" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>